<commit_message>
Changes made to version from 18 to 17
</commit_message>
<xml_diff>
--- a/Group5 Individual Assessment.xlsx
+++ b/Group5 Individual Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puter\IdeaProjects\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04F2C81-6434-4F22-9F29-3DD48312C8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545DA37C-40A3-4724-B5D0-E31E2835A645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{81577C34-F628-4BE4-9909-E14FB6C69AA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{81577C34-F628-4BE4-9909-E14FB6C69AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,12 +209,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -540,42 +539,39 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
         <v>40582939</v>
       </c>
       <c r="C3" s="2">
@@ -586,71 +582,59 @@
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="8">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
         <v>40598611</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="8">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
         <v>40578064</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="8">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
         <v>40542238</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="8">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
         <v>40533866</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>100</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>100</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>100</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>100</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
for Code Review 3
</commit_message>
<xml_diff>
--- a/Group5 Individual Assessment.xlsx
+++ b/Group5 Individual Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puter\IdeaProjects\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\school of computing\user data\40598611\My Profile\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545DA37C-40A3-4724-B5D0-E31E2835A645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF5F3AC-A8C1-4BE9-8CB8-257CDD052A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{81577C34-F628-4BE4-9909-E14FB6C69AA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{81577C34-F628-4BE4-9909-E14FB6C69AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -92,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -205,11 +204,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -222,6 +230,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,28 +550,28 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -570,65 +581,93 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <v>40582939</v>
       </c>
       <c r="C3" s="2">
         <v>20</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>40598611</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
+      <c r="D4" s="14">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14">
+        <v>20</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>40578064</v>
       </c>
       <c r="C5">
         <v>20</v>
       </c>
+      <c r="D5" s="14">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14">
+        <v>20</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>40542238</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
+      <c r="D6" s="14">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14">
+        <v>20</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>40533866</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
+      <c r="D7" s="13">
+        <v>20</v>
+      </c>
+      <c r="E7" s="13">
+        <v>20</v>
+      </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9">
         <v>100</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="13">
         <v>100</v>
       </c>
       <c r="F8" s="10">

</xml_diff>